<commit_message>
Final Version before Presentation on 3rd Dec
</commit_message>
<xml_diff>
--- a/As-Is/Result/Road Usage.xlsx
+++ b/As-Is/Result/Road Usage.xlsx
@@ -374,619 +374,982 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A122"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>106</v>
+      </c>
+      <c r="B2">
         <v>1535</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>107</v>
+      </c>
+      <c r="B3">
         <v>782</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>64</v>
+      </c>
+      <c r="B4">
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>51</v>
+      </c>
+      <c r="B5">
         <v>588</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>53</v>
+      </c>
+      <c r="B6">
         <v>495</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>52</v>
+      </c>
+      <c r="B7">
         <v>816</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>55</v>
+      </c>
+      <c r="B8">
         <v>816</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>54</v>
+      </c>
+      <c r="B9">
         <v>816</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>57</v>
+      </c>
+      <c r="B10">
         <v>1134</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11">
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>58</v>
+      </c>
+      <c r="B11">
         <v>1134</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12">
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>61</v>
+      </c>
+      <c r="B12">
         <v>1015</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13">
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>60</v>
+      </c>
+      <c r="B13">
         <v>1015</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14">
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>116</v>
+      </c>
+      <c r="B14">
         <v>2417</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15">
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>114</v>
+      </c>
+      <c r="B15">
         <v>2417</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16">
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>115</v>
+      </c>
+      <c r="B16">
         <v>2350</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>159</v>
+      </c>
+      <c r="B17">
         <v>377</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18">
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>117</v>
+      </c>
+      <c r="B18">
         <v>2446</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19">
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>122</v>
+      </c>
+      <c r="B19">
         <v>2966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20">
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>78</v>
+      </c>
+      <c r="B20">
         <v>4402</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21">
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>77</v>
+      </c>
+      <c r="B21">
         <v>2747</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22">
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>91</v>
+      </c>
+      <c r="B22">
         <v>2747</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23">
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>90</v>
+      </c>
+      <c r="B23">
         <v>2897</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24">
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>93</v>
+      </c>
+      <c r="B24">
         <v>2897</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25">
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>94</v>
+      </c>
+      <c r="B25">
         <v>2552</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26">
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>95</v>
+      </c>
+      <c r="B26">
         <v>2552</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27">
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>96</v>
+      </c>
+      <c r="B27">
         <v>2552</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28">
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>92</v>
+      </c>
+      <c r="B28">
         <v>2972</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29">
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>97</v>
+      </c>
+      <c r="B29">
         <v>2972</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30">
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>99</v>
+      </c>
+      <c r="B30">
         <v>2972</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31">
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>100</v>
+      </c>
+      <c r="B31">
         <v>2972</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32">
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>101</v>
+      </c>
+      <c r="B32">
         <v>2974</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33">
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>102</v>
+      </c>
+      <c r="B33">
         <v>2974</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34">
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>98</v>
+      </c>
+      <c r="B34">
         <v>3431</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35">
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>151</v>
+      </c>
+      <c r="B35">
         <v>3431</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36">
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>152</v>
+      </c>
+      <c r="B36">
         <v>2914</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37">
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>123</v>
+      </c>
+      <c r="B37">
         <v>2741</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38">
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>118</v>
+      </c>
+      <c r="B38">
         <v>2774</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39">
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>121</v>
+      </c>
+      <c r="B39">
         <v>3070</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40">
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>86</v>
+      </c>
+      <c r="B40">
         <v>3166</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41">
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>87</v>
+      </c>
+      <c r="B41">
         <v>3184</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
-      <c r="A42">
+    <row r="42" spans="1:2">
+      <c r="A42" s="1">
+        <v>124</v>
+      </c>
+      <c r="B42">
         <v>709</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43">
+    <row r="43" spans="1:2">
+      <c r="A43" s="1">
+        <v>125</v>
+      </c>
+      <c r="B43">
         <v>410</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44">
+    <row r="44" spans="1:2">
+      <c r="A44" s="1">
+        <v>126</v>
+      </c>
+      <c r="B44">
         <v>391</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45">
+    <row r="45" spans="1:2">
+      <c r="A45" s="1">
+        <v>68</v>
+      </c>
+      <c r="B45">
         <v>391</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46">
+    <row r="46" spans="1:2">
+      <c r="A46" s="1">
+        <v>72</v>
+      </c>
+      <c r="B46">
         <v>391</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47">
+    <row r="47" spans="1:2">
+      <c r="A47" s="1">
+        <v>70</v>
+      </c>
+      <c r="B47">
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48">
+    <row r="48" spans="1:2">
+      <c r="A48" s="1">
+        <v>71</v>
+      </c>
+      <c r="B48">
         <v>393</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49">
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>69</v>
+      </c>
+      <c r="B49">
         <v>393</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50">
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
+        <v>47</v>
+      </c>
+      <c r="B50">
         <v>1056</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51">
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
+        <v>46</v>
+      </c>
+      <c r="B51">
         <v>1056</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52">
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>48</v>
+      </c>
+      <c r="B52">
         <v>1425</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53">
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>49</v>
+      </c>
+      <c r="B53">
         <v>1425</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54">
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>37</v>
+      </c>
+      <c r="B54">
         <v>2411</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55">
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>148</v>
+      </c>
+      <c r="B55">
         <v>3082</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56">
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>149</v>
+      </c>
+      <c r="B56">
         <v>3082</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57">
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>80</v>
+      </c>
+      <c r="B57">
         <v>4243</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58">
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>27</v>
+      </c>
+      <c r="B58">
         <v>2883</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59">
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>28</v>
+      </c>
+      <c r="B59">
         <v>2853</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60">
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>41</v>
+      </c>
+      <c r="B60">
         <v>9972</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61">
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>40</v>
+      </c>
+      <c r="B61">
         <v>9085</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62">
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>43</v>
+      </c>
+      <c r="B62">
         <v>9085</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63">
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>42</v>
+      </c>
+      <c r="B63">
         <v>7997</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64">
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>39</v>
+      </c>
+      <c r="B64">
         <v>7997</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65">
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>38</v>
+      </c>
+      <c r="B65">
         <v>7516</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66">
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>105</v>
+      </c>
+      <c r="B66">
         <v>1376</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67">
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>113</v>
+      </c>
+      <c r="B67">
         <v>1376</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68">
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>85</v>
+      </c>
+      <c r="B68">
         <v>3535</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69">
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>84</v>
+      </c>
+      <c r="B69">
         <v>3535</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70">
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>81</v>
+      </c>
+      <c r="B70">
         <v>3512</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71">
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>82</v>
+      </c>
+      <c r="B71">
         <v>3339</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72">
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>83</v>
+      </c>
+      <c r="B72">
         <v>3339</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73">
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
+        <v>79</v>
+      </c>
+      <c r="B73">
         <v>3507</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74">
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
+        <v>75</v>
+      </c>
+      <c r="B74">
         <v>676</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75">
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
         <v>690</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76">
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
+        <v>127</v>
+      </c>
+      <c r="B76">
         <v>629</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77">
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>128</v>
+      </c>
+      <c r="B77">
         <v>550</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78">
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>74</v>
+      </c>
+      <c r="B78">
         <v>765</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79">
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>129</v>
+      </c>
+      <c r="B79">
         <v>249</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80">
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
+        <v>66</v>
+      </c>
+      <c r="B80">
         <v>284</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
-      <c r="A81">
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
+        <v>65</v>
+      </c>
+      <c r="B81">
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
-      <c r="A82">
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>63</v>
+      </c>
+      <c r="B82">
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83">
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>62</v>
+      </c>
+      <c r="B83">
         <v>282</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
-      <c r="A84">
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>44</v>
+      </c>
+      <c r="B84">
         <v>7595</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
-      <c r="A85">
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>45</v>
+      </c>
+      <c r="B85">
         <v>7857</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86">
+    <row r="86" spans="1:2">
+      <c r="A86" s="1">
+        <v>14</v>
+      </c>
+      <c r="B86">
         <v>7833</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
-      <c r="A87">
+    <row r="87" spans="1:2">
+      <c r="A87" s="1">
+        <v>13</v>
+      </c>
+      <c r="B87">
         <v>7889</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
-      <c r="A88">
+    <row r="88" spans="1:2">
+      <c r="A88" s="1">
+        <v>12</v>
+      </c>
+      <c r="B88">
         <v>7889</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
-      <c r="A89">
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>76</v>
+      </c>
+      <c r="B89">
         <v>575</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90">
+    <row r="90" spans="1:2">
+      <c r="A90" s="1">
+        <v>36</v>
+      </c>
+      <c r="B90">
         <v>1364</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91">
+    <row r="91" spans="1:2">
+      <c r="A91" s="1">
+        <v>120</v>
+      </c>
+      <c r="B91">
         <v>386</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92">
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>135</v>
+      </c>
+      <c r="B92">
         <v>133</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93">
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>150</v>
+      </c>
+      <c r="B93">
         <v>991</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94">
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>142</v>
+      </c>
+      <c r="B94">
         <v>991</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95">
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>158</v>
+      </c>
+      <c r="B95">
         <v>817</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96">
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>24</v>
+      </c>
+      <c r="B96">
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97">
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>108</v>
+      </c>
+      <c r="B97">
         <v>380</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98">
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>109</v>
+      </c>
+      <c r="B98">
         <v>380</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99">
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>110</v>
+      </c>
+      <c r="B99">
         <v>374</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
-      <c r="A100">
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>111</v>
+      </c>
+      <c r="B100">
         <v>346</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
-      <c r="A101">
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>11</v>
+      </c>
+      <c r="B101">
         <v>5855</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
-      <c r="A102">
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>16</v>
+      </c>
+      <c r="B102">
         <v>122</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
-      <c r="A103">
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>103</v>
+      </c>
+      <c r="B103">
         <v>507</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104">
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>139</v>
+      </c>
+      <c r="B104">
         <v>5937</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105">
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>23</v>
+      </c>
+      <c r="B105">
         <v>6076</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
-      <c r="A106">
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>25</v>
+      </c>
+      <c r="B106">
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107">
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>31</v>
+      </c>
+      <c r="B107">
         <v>99</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
-      <c r="A108">
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>30</v>
+      </c>
+      <c r="B108">
         <v>99</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
-      <c r="A109">
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>133</v>
+      </c>
+      <c r="B109">
         <v>155</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
-      <c r="A110">
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>35</v>
+      </c>
+      <c r="B110">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
-      <c r="A111">
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>29</v>
+      </c>
+      <c r="B111">
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
-      <c r="A112">
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>17</v>
+      </c>
+      <c r="B112">
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113">
+    <row r="113" spans="1:2">
+      <c r="A113" s="1">
+        <v>18</v>
+      </c>
+      <c r="B113">
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
-      <c r="A114">
+    <row r="114" spans="1:2">
+      <c r="A114" s="1">
+        <v>19</v>
+      </c>
+      <c r="B114">
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
-      <c r="A115">
+    <row r="115" spans="1:2">
+      <c r="A115" s="1">
+        <v>20</v>
+      </c>
+      <c r="B115">
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
-      <c r="A116">
+    <row r="116" spans="1:2">
+      <c r="A116" s="1">
+        <v>21</v>
+      </c>
+      <c r="B116">
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
-      <c r="A117">
+    <row r="117" spans="1:2">
+      <c r="A117" s="1">
+        <v>8</v>
+      </c>
+      <c r="B117">
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
-      <c r="A118">
+    <row r="118" spans="1:2">
+      <c r="A118" s="1">
+        <v>9</v>
+      </c>
+      <c r="B118">
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
-      <c r="A119">
+    <row r="119" spans="1:2">
+      <c r="A119" s="1">
+        <v>144</v>
+      </c>
+      <c r="B119">
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
-      <c r="A120">
+    <row r="120" spans="1:2">
+      <c r="A120" s="1">
+        <v>22</v>
+      </c>
+      <c r="B120">
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
-      <c r="A121">
+    <row r="121" spans="1:2">
+      <c r="A121" s="1">
+        <v>154</v>
+      </c>
+      <c r="B121">
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
-      <c r="A122">
+    <row r="122" spans="1:2">
+      <c r="A122" s="1">
+        <v>156</v>
+      </c>
+      <c r="B122">
         <v>4</v>
       </c>
     </row>

</xml_diff>